<commit_message>
added order details of 14-06-2018
</commit_message>
<xml_diff>
--- a/fb marketplace/orders/June 2018/order.tracker_jun2018.xlsx
+++ b/fb marketplace/orders/June 2018/order.tracker_jun2018.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Customer Name</t>
   </si>
@@ -86,54 +86,12 @@
     <t>Sold Price</t>
   </si>
   <si>
-    <t>Sushil Joglekar</t>
-  </si>
-  <si>
-    <t>Raj Kishore</t>
-  </si>
-  <si>
-    <t>Mir Mukkaram</t>
-  </si>
-  <si>
-    <t>Prashant Singh</t>
-  </si>
-  <si>
-    <t>Mithilesh KumarSingh</t>
-  </si>
-  <si>
-    <t>Atish Dash</t>
-  </si>
-  <si>
-    <t>Sravan Ganesh Chary</t>
-  </si>
-  <si>
-    <t>Ranaveer Mamidi</t>
-  </si>
-  <si>
     <t>Not Interested</t>
   </si>
   <si>
-    <t>Sai Sumanth</t>
-  </si>
-  <si>
-    <t>Prabhakar Begari</t>
-  </si>
-  <si>
-    <t>Srinivas Ravindra Velagapudi</t>
-  </si>
-  <si>
     <t>Sold Date</t>
   </si>
   <si>
-    <t>Sai Chakravarthi</t>
-  </si>
-  <si>
-    <t>Renamala PranayKumar</t>
-  </si>
-  <si>
-    <t>Phani Vuppula</t>
-  </si>
-  <si>
     <t>Mobile Number</t>
   </si>
   <si>
@@ -146,25 +104,22 @@
     <t>Additional Shipping</t>
   </si>
   <si>
-    <t>Ghouse Pasha</t>
-  </si>
-  <si>
-    <t>Lucky Royals</t>
-  </si>
-  <si>
-    <t>Sunny Abhimanyu Sharma</t>
-  </si>
-  <si>
-    <t>Abhilash Hindu</t>
-  </si>
-  <si>
-    <t>Shiva Rock</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Dpr Prem</t>
+    <t>Ravi Kumar</t>
+  </si>
+  <si>
+    <t>Gimto Smart Watch</t>
+  </si>
+  <si>
+    <t>Tech Mahindra near Shilparamam</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Was sensible and pleasant customer, so gave him free shipping</t>
   </si>
 </sst>
 </file>
@@ -206,9 +161,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +489,7 @@
         <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -545,24 +501,24 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="M1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="N1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -571,404 +527,34 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>3499</v>
+        <v>1499</v>
+      </c>
+      <c r="F2">
+        <v>1499</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43265</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>3499</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>3499</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>3499</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>3499</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>3499</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>3499</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>3499</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10">
-        <v>3499</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>3499</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>1499</v>
-      </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2">
+        <v>9885447656</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>1499</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="N2" t="s">
         <v>31</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>1499</v>
-      </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <v>1499</v>
-      </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16">
-        <v>749</v>
-      </c>
-      <c r="H16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <v>749</v>
-      </c>
-      <c r="H17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>749</v>
-      </c>
-      <c r="H18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19">
-        <v>749</v>
-      </c>
-      <c r="H19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20">
-        <v>749</v>
-      </c>
-      <c r="H20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22">
-        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +582,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Items!$A$1:$A$6</xm:f>
+            <xm:f>Items!$A$1:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -1045,7 +631,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1055,10 +641,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,6 +700,14 @@
         <v>385</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>1499</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>